<commit_message>
Categorization added with stored json
</commit_message>
<xml_diff>
--- a/expenses.xlsx
+++ b/expenses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,7 +571,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>miscellaneous</t>
+          <t>Food &amp; Necessities</t>
         </is>
       </c>
     </row>
@@ -691,7 +691,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>miscellaneous</t>
+          <t>Food &amp; Necessities</t>
         </is>
       </c>
     </row>
@@ -711,7 +711,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>miscellaneous</t>
+          <t>Miscellaneous</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>miscellaneous</t>
+          <t>Food &amp; Necessities</t>
         </is>
       </c>
     </row>
@@ -931,7 +931,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>miscellaneous</t>
+          <t>Food &amp; Necessities</t>
         </is>
       </c>
     </row>
@@ -971,7 +971,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>miscellaneous</t>
+          <t>Food &amp; Necessities</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>miscellaneous</t>
+          <t>Entertainment</t>
         </is>
       </c>
     </row>
@@ -1230,6 +1230,46 @@
         </is>
       </c>
       <c r="D40" t="inlineStr">
+        <is>
+          <t>Food &amp; Necessities</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>1.12.24</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>300</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>misc</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Miscellaneous</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>30.11.24</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>500</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>coconut</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
         <is>
           <t>Food &amp; Necessities</t>
         </is>

</xml_diff>

<commit_message>
Read from txt, insights support added
</commit_message>
<xml_diff>
--- a/expenses.xlsx
+++ b/expenses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -818,20 +818,20 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>29.11.24</t>
+          <t>30.11.24</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>pohe</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Miscellaneous</t>
+          <t>Food &amp; Necessities</t>
         </is>
       </c>
     </row>
@@ -842,16 +842,16 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>25</v>
+        <v>473</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>pohe</t>
+          <t>healthy things grocery</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Food &amp; Necessities</t>
+          <t>Personal Care</t>
         </is>
       </c>
     </row>
@@ -862,36 +862,36 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>473</v>
+        <v>80</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>healthy things grocery</t>
+          <t>paneer and veggie</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Personal Care</t>
+          <t>Food &amp; Necessities</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>30.11.24</t>
+          <t>1.12.24</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>80</v>
+        <v>300</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>paneer and veggie</t>
+          <t>petrol</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Food &amp; Necessities</t>
+          <t>Transportation</t>
         </is>
       </c>
     </row>
@@ -902,16 +902,16 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>300</v>
+        <v>30</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>petrol</t>
+          <t>pinapple juice from piyush, gore ðŸ”´ðŸ”´</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Transportation</t>
+          <t>Miscellaneous</t>
         </is>
       </c>
     </row>
@@ -922,11 +922,11 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>30</v>
+        <v>166</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>pinapple juice from piyush, gore 🔴🔴</t>
+          <t>dinner</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -942,11 +942,11 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>166</v>
+        <v>790</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>dinner</t>
+          <t>harmosa eats</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -962,16 +962,16 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>790</v>
+        <v>450</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>harmosa eats</t>
+          <t>maid</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Food &amp; Necessities</t>
+          <t>Rent &amp; Bills</t>
         </is>
       </c>
     </row>
@@ -982,36 +982,36 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>450</v>
+        <v>6250</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>maid</t>
+          <t>rent</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Rent &amp; Bills</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1.12.24</t>
+          <t>2.12.24</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>6250</v>
+        <v>199</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>rent</t>
+          <t>Netflix</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Entertainment</t>
         </is>
       </c>
     </row>
@@ -1022,16 +1022,16 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>199</v>
+        <v>151</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Netflix</t>
+          <t>rice, aata</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Food &amp; Necessities</t>
         </is>
       </c>
     </row>
@@ -1042,11 +1042,11 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>rice, aata</t>
+          <t>dinner</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1058,15 +1058,15 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2.12.24</t>
+          <t>3.12.24</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>150</v>
+        <v>70</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>dinner</t>
+          <t>paratha</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1082,11 +1082,11 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>paratha</t>
+          <t>dinner</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1098,15 +1098,15 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>3.12.24</t>
+          <t>4.12.24</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>dinner</t>
+          <t>lunch</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1122,11 +1122,11 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>111</v>
+        <v>141</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>lunch</t>
+          <t>dinner</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1138,20 +1138,20 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>4.12.24</t>
+          <t>6.12.24</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>141</v>
+        <v>214</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>dinner</t>
+          <t>electricity bill</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Food &amp; Necessities</t>
+          <t>Rent &amp; Bills</t>
         </is>
       </c>
     </row>
@@ -1162,114 +1162,34 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>214</v>
+        <v>38</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>electricity bill</t>
+          <t>cab for party</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Transportation</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6.12.24</t>
+          <t>7.12.24</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>cab for party</t>
+          <t>lunch</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
-        <is>
-          <t>Transportation</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>6.12.24</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>34</v>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>misc</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Miscellaneous</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>7.12.24</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>77</v>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>lunch</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Food &amp; Necessities</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>1.12.24</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
-        <v>300</v>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>misc</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Miscellaneous</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>30.11.24</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>500</v>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>coconut</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
         <is>
           <t>Food &amp; Necessities</t>
         </is>

</xml_diff>